<commit_message>
Rerun some analyses with more data
</commit_message>
<xml_diff>
--- a/data/descriptives/dataset_year.xlsx
+++ b/data/descriptives/dataset_year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anuschka/Documents/climatechange/climatechange/data/descriptives/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\climatechange\data\descriptives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF91CA4-98EA-F445-A34D-DEFA8F156407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F0542E-C9B3-4D45-B1F3-C256BF2288C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="15620" xr2:uid="{0EA7B5FD-2E99-6A4D-A703-5D6476F60236}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0EA7B5FD-2E99-6A4D-A703-5D6476F60236}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="20">
   <si>
     <t>dataset</t>
   </si>
@@ -78,6 +78,24 @@
   </si>
   <si>
     <t>#F1C40F</t>
+  </si>
+  <si>
+    <t>MOT</t>
+  </si>
+  <si>
+    <t>SOCON</t>
+  </si>
+  <si>
+    <t>LISS</t>
+  </si>
+  <si>
+    <t>#E02023</t>
+  </si>
+  <si>
+    <t>#1676E3</t>
+  </si>
+  <si>
+    <t>#0AC760</t>
   </si>
 </sst>
 </file>
@@ -123,7 +141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -139,7 +157,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -435,15 +453,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1007F5BD-8742-3446-8AA2-A93523ABA8BC}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,7 +475,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -471,7 +489,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -485,7 +503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -499,7 +517,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -513,7 +531,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -527,7 +545,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -541,7 +559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -555,7 +573,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -569,7 +587,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -583,7 +601,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -597,7 +615,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -611,7 +629,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -625,7 +643,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -639,7 +657,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -653,7 +671,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -667,7 +685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -681,7 +699,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -695,7 +713,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -709,7 +727,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -723,7 +741,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -737,7 +755,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -751,7 +769,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -765,7 +783,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -779,7 +797,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -791,6 +809,132 @@
       </c>
       <c r="D25" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>2019</v>
+      </c>
+      <c r="D26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>2021</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>2020</v>
+      </c>
+      <c r="D28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>2021</v>
+      </c>
+      <c r="D29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>2022</v>
+      </c>
+      <c r="D30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>2019</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>2020</v>
+      </c>
+      <c r="D32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>2020</v>
+      </c>
+      <c r="D33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>2021</v>
+      </c>
+      <c r="D34" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>